<commit_message>
metainformacion de la provincia con el número
</commit_message>
<xml_diff>
--- a/input/data/calidad del aire/provincia con numero.xlsx
+++ b/input/data/calidad del aire/provincia con numero.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25917"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CALIDAD DEL AIRE\Base de Datos\Peticiones_información\DATOS_completos_web\2019\conMatadero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7992047C-590E-40B2-AB67-6403E14B6DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D4A0088-55D4-426C-84CE-3E2E50AB6A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12435" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>